<commit_message>
Configuration items list document Version 1.0
</commit_message>
<xml_diff>
--- a/CAR_CI List.xlsx
+++ b/CAR_CI List.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="40">
   <si>
     <t>Folder</t>
   </si>
@@ -126,7 +126,16 @@
     <t>Document contains questions about requirements with Proposal and customer's answers.</t>
   </si>
   <si>
-    <t>It is a document that outlines what work needs to be done, the order in which it needs to be done, what resources are required, how they will be distributed, and how long different parts of the work will take.</t>
+    <t>The project schedule is the tool that communicates what work needs to be performed, which resources of the organization will perform the work and the timeframes in which that work needs to be performed.</t>
+  </si>
+  <si>
+    <t>work breakdown structure</t>
+  </si>
+  <si>
+    <t>CAR_work breakdown structure</t>
+  </si>
+  <si>
+    <t>WBS is a key project deliverable that organizes the team's work into manageable sections</t>
   </si>
 </sst>
 </file>
@@ -245,11 +254,11 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -556,10 +565,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B15" sqref="A15:XFD15"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.140625" defaultRowHeight="47.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -591,7 +600,7 @@
       <c r="A3" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="10">
+      <c r="B3" s="9">
         <v>43470</v>
       </c>
     </row>
@@ -628,7 +637,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="10" t="s">
         <v>15</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -645,7 +654,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="9"/>
+      <c r="A9" s="10"/>
       <c r="B9" s="1" t="s">
         <v>4</v>
       </c>
@@ -660,7 +669,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="9"/>
+      <c r="A10" s="10"/>
       <c r="B10" s="1" t="s">
         <v>5</v>
       </c>
@@ -675,7 +684,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="9"/>
+      <c r="A11" s="10"/>
       <c r="B11" s="1" t="s">
         <v>6</v>
       </c>
@@ -690,7 +699,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="9"/>
+      <c r="A12" s="10"/>
       <c r="B12" s="1" t="s">
         <v>7</v>
       </c>
@@ -705,7 +714,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="9"/>
+      <c r="A13" s="10"/>
       <c r="B13" s="1" t="s">
         <v>8</v>
       </c>
@@ -720,7 +729,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="9"/>
+      <c r="A14" s="10"/>
       <c r="B14" s="3" t="s">
         <v>21</v>
       </c>
@@ -735,7 +744,7 @@
       </c>
     </row>
     <row r="15" spans="1:5" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="9"/>
+      <c r="A15" s="10"/>
       <c r="B15" s="3" t="s">
         <v>22</v>
       </c>
@@ -749,9 +758,24 @@
         <v>16</v>
       </c>
     </row>
+    <row r="16" spans="1:5" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="10"/>
+      <c r="B16" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A8:A15"/>
+    <mergeCell ref="A8:A16"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B8" r:id="rId1" tooltip="CAR_Issues and Risks_V1.0.xlsx" display="https://github.com/FatmaMohamedSoliman/CarPurchasing/blob/Documents/CAR_Issues and Risks_V1.0.xlsx"/>

</xml_diff>

<commit_message>
Configuration item list Version 1.1
add 3 documents with their description
</commit_message>
<xml_diff>
--- a/CAR_CI List.xlsx
+++ b/CAR_CI List.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="50">
   <si>
     <t>Folder</t>
   </si>
@@ -105,9 +105,6 @@
     <t>Approval Date</t>
   </si>
   <si>
-    <t>Description of Change</t>
-  </si>
-  <si>
     <t>Fatma mohamed</t>
   </si>
   <si>
@@ -136,6 +133,39 @@
   </si>
   <si>
     <t>WBS is a key project deliverable that organizes the team's work into manageable sections</t>
+  </si>
+  <si>
+    <t>Sara Ibrahim</t>
+  </si>
+  <si>
+    <t>RACI</t>
+  </si>
+  <si>
+    <t>Configuratin management plan</t>
+  </si>
+  <si>
+    <t>CAR_CM PLANS</t>
+  </si>
+  <si>
+    <t>CAR_CI List</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Configuratin Item list </t>
+  </si>
+  <si>
+    <t>SRS peer reviwe sheet</t>
+  </si>
+  <si>
+    <t>CAR_SRS_PR_Sheet</t>
+  </si>
+  <si>
+    <t>A document that contains a reviewer's observations on SRS document</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Document contains all documents uploaded on GitHub with there id and description </t>
+  </si>
+  <si>
+    <t>Document contains purpose of CM, approach and Configuration Identification.</t>
   </si>
 </sst>
 </file>
@@ -565,10 +595,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.140625" defaultRowHeight="47.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -593,7 +623,7 @@
         <v>25</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -608,75 +638,91 @@
       <c r="A4" s="7" t="s">
         <v>27</v>
       </c>
+      <c r="B4" s="1" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="5" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="B5" s="9">
+        <v>43501</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B6" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
+    <row r="7" spans="1:5" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B7" s="3" t="s">
         <v>19</v>
       </c>
+      <c r="C7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="10"/>
+      <c r="B8" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="C8" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>20</v>
+        <v>9</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>32</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10"/>
       <c r="B9" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>33</v>
+        <v>10</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>30</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10"/>
       <c r="B10" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>31</v>
       </c>
       <c r="E10" s="1" t="s">
@@ -686,13 +732,13 @@
     <row r="11" spans="1:5" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10"/>
       <c r="B11" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>16</v>
@@ -701,58 +747,58 @@
     <row r="12" spans="1:5" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10"/>
       <c r="B12" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10"/>
-      <c r="B13" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>13</v>
+      <c r="B13" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10"/>
       <c r="B14" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="10"/>
-      <c r="B15" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>23</v>
+      <c r="B15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>16</v>
@@ -761,30 +807,61 @@
     <row r="16" spans="1:5" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10"/>
       <c r="B16" s="1" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="E16" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="10"/>
+      <c r="B17" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="10"/>
+      <c r="B18" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>16</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A8:A16"/>
+    <mergeCell ref="A7:A18"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B8" r:id="rId1" tooltip="CAR_Issues and Risks_V1.0.xlsx" display="https://github.com/FatmaMohamedSoliman/CarPurchasing/blob/Documents/CAR_Issues and Risks_V1.0.xlsx"/>
-    <hyperlink ref="C14" r:id="rId2" tooltip="CAR_RACI.xlsx" display="https://github.com/FatmaMohamedSoliman/CarPurchasing/blob/Documents/CAR_RACI.xlsx"/>
-    <hyperlink ref="B15" r:id="rId3" tooltip="Project Schedule Version 1.0" display="https://github.com/FatmaMohamedSoliman/CarPurchasing/commit/18ca75c6f871fc1f88bbbc41280f7c96c4d9375a"/>
-    <hyperlink ref="C15" r:id="rId4" tooltip="CAR_Project_Schedule.xlsx" display="https://github.com/FatmaMohamedSoliman/CarPurchasing/blob/Documents/CAR_Project_Schedule.xlsx"/>
-    <hyperlink ref="B14" r:id="rId5" tooltip="CAR_RACI.xlsx" display="https://github.com/FatmaMohamedSoliman/CarPurchasing/blob/Documents/CAR_RACI.xlsx"/>
+    <hyperlink ref="B7" r:id="rId1" tooltip="CAR_Issues and Risks_V1.0.xlsx" display="https://github.com/FatmaMohamedSoliman/CarPurchasing/blob/Documents/CAR_Issues and Risks_V1.0.xlsx"/>
+    <hyperlink ref="C13" r:id="rId2" tooltip="CAR_RACI.xlsx" display="https://github.com/FatmaMohamedSoliman/CarPurchasing/blob/Documents/CAR_RACI.xlsx"/>
+    <hyperlink ref="B14" r:id="rId3" tooltip="Project Schedule Version 1.0" display="https://github.com/FatmaMohamedSoliman/CarPurchasing/commit/18ca75c6f871fc1f88bbbc41280f7c96c4d9375a"/>
+    <hyperlink ref="C14" r:id="rId4" tooltip="CAR_Project_Schedule.xlsx" display="https://github.com/FatmaMohamedSoliman/CarPurchasing/blob/Documents/CAR_Project_Schedule.xlsx"/>
+    <hyperlink ref="B13" r:id="rId5" tooltip="CAR_RACI.xlsx" display="https://github.com/FatmaMohamedSoliman/CarPurchasing/blob/Documents/CAR_RACI.xlsx"/>
+    <hyperlink ref="C18" r:id="rId6" tooltip="CAR_SRS_PR_Sheet.doc" display="https://github.com/FatmaMohamedSoliman/CarPurchasing/blob/Documents/CAR_SRS_PR_Sheet.doc"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>